<commit_message>
changing the format of levenshtein, new mapping
</commit_message>
<xml_diff>
--- a/digitized data/metadatalocation.xlsx
+++ b/digitized data/metadatalocation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis/VAULTS/BA THESIS/Codes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5E09778-99EF-9B4D-BC59-338693AB5737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C25D5FA-5A49-0E45-A86F-B53F5CAC54D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="620" windowWidth="26740" windowHeight="16340" xr2:uid="{382D2112-BF2B-A04A-84E3-B923D635D9ED}"/>
+    <workbookView xWindow="540" yWindow="1120" windowWidth="26340" windowHeight="15840" xr2:uid="{7A5E0C24-EC50-BF4E-A0C6-90F8CD4A6738}"/>
   </bookViews>
   <sheets>
     <sheet name="metadatalocation" sheetId="1" r:id="rId1"/>
@@ -930,7 +930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244086EB-B95C-BC48-9DD7-27E0FC36AD4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66916B8D-182A-3345-A367-092950833031}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>